<commit_message>
version 1.4 of the board
</commit_message>
<xml_diff>
--- a/RoverWingBoard/BOM-V1.0.xlsx
+++ b/RoverWingBoard/BOM-V1.0.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shurik\Dropbox\Robotics\RoverWing\RoverWingHardware\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shurik\Dropbox\Robotics\RoverWing\RoverWingHardware\RoverWingBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEA6C1E-5D97-4D2F-BB25-60CEA7B7D2BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDECA147-1B68-4A0A-A81C-C4EE202E07A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM-v1.0" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM-v1.3" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="260">
   <si>
     <t>Qty</t>
   </si>
@@ -793,6 +796,21 @@
   </si>
   <si>
     <t>HEADER-3X06</t>
+  </si>
+  <si>
+    <t>1.5k</t>
+  </si>
+  <si>
+    <t>5.49k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 1.5K OHMs Â±5% 1/8W </t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>R13,R14,R15,R16</t>
   </si>
 </sst>
 </file>
@@ -1654,7 +1672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+    <sheetView topLeftCell="B13" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -3190,4 +3208,1526 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB74638-E99E-46EA-A319-8B0B03B0C841}">
+  <dimension ref="A1:M41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.81640625" style="1"/>
+    <col min="2" max="2" width="3.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.90625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" style="1"/>
+    <col min="7" max="7" width="14.6328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.26953125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" style="1"/>
+    <col min="12" max="12" width="29.453125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="1">
+        <f>K2*B2</f>
+        <v>7.2499999999999995E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1">
+        <v>50</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1.52E-2</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" ref="M3:M36" si="0">K3*B3</f>
+        <v>1.52E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1">
+        <v>50</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1.35E-2</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" si="0"/>
+        <v>1.35E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="1">
+        <v>5</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.12239999999999999</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.36719999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="1">
+        <v>50</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.16899999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="1">
+        <v>50</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1.23E-2</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.23E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="1">
+        <v>20</v>
+      </c>
+      <c r="K8" s="1">
+        <v>2.0299999999999999E-2</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="0"/>
+        <v>6.0899999999999996E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="1">
+        <v>20</v>
+      </c>
+      <c r="K9" s="1">
+        <v>2.76E-2</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="0"/>
+        <v>2.76E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="1">
+        <v>20</v>
+      </c>
+      <c r="K10" s="1">
+        <v>3.5099999999999999E-2</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="0"/>
+        <v>3.5099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="J11" s="1">
+        <v>5</v>
+      </c>
+      <c r="K11" s="1">
+        <v>6.6799999999999998E-2</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.20039999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="1">
+        <v>5</v>
+      </c>
+      <c r="K12" s="1">
+        <v>9.9699999999999997E-2</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="0"/>
+        <v>9.9699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.1454</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1454</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.1201</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.26550000000000001</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.26550000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="1">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="J19" s="1">
+        <v>10</v>
+      </c>
+      <c r="K19" s="1">
+        <v>5.91E-2</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41370000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J20" s="1">
+        <v>10</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.1082</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1082</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J21" s="1">
+        <v>5</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.1145</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J22" s="1">
+        <v>50</v>
+      </c>
+      <c r="K22" s="1">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J23" s="1">
+        <v>100</v>
+      </c>
+      <c r="K23" s="1">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="J24" s="1">
+        <v>50</v>
+      </c>
+      <c r="K24" s="1">
+        <v>3.8E-3</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="0"/>
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J25" s="1">
+        <v>50</v>
+      </c>
+      <c r="K25" s="1">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="0"/>
+        <v>8.0999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="1">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="J27" s="1">
+        <v>50</v>
+      </c>
+      <c r="K27" s="1">
+        <v>4.3E-3</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="M27" s="1">
+        <f t="shared" si="0"/>
+        <v>1.29E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J28" s="1">
+        <v>20</v>
+      </c>
+      <c r="K28" s="1">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="M28" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="J29" s="1">
+        <v>1</v>
+      </c>
+      <c r="K29" s="1">
+        <v>3.22</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="M29" s="1">
+        <f t="shared" si="0"/>
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="J30" s="1">
+        <v>10</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0.32140000000000002</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="M30" s="1">
+        <f t="shared" si="0"/>
+        <v>0.32140000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="J31" s="1">
+        <v>5</v>
+      </c>
+      <c r="K31" s="1">
+        <v>8.1299999999999997E-2</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="M31" s="1">
+        <f t="shared" si="0"/>
+        <v>8.1299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="J32" s="1">
+        <v>1</v>
+      </c>
+      <c r="K32" s="1">
+        <v>2.8835000000000002</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="M32" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8835000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="J33" s="1">
+        <v>1</v>
+      </c>
+      <c r="K33" s="1">
+        <v>1.7250000000000001</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="M33" s="1">
+        <f t="shared" si="0"/>
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="J34" s="1">
+        <v>1</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0.69340000000000002</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="M34" s="1">
+        <f t="shared" si="0"/>
+        <v>0.69340000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="J35" s="1">
+        <v>5</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0.12809999999999999</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="M35" s="1">
+        <f t="shared" si="0"/>
+        <v>0.12809999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="J36" s="1">
+        <v>1</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="M36" s="1">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L37" s="2"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>